<commit_message>
2021 Mar 1 release
</commit_message>
<xml_diff>
--- a/analyses/knowledge-bases/target/almanac-comparison.xlsx
+++ b/analyses/knowledge-bases/target/almanac-comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendan/Github/moalmanac-paper/sources/target/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendan/Github/moalmanac-paper/analyses/knowledge-bases/target/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFB51C9-94F9-D847-9AA3-971BE4B9E808}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB85D46C-5842-744E-96C6-5DDEB1D3A4AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="5660" windowWidth="36940" windowHeight="12460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1600" windowWidth="28800" windowHeight="16140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Supp_Table_3_Actionable_genes_r" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="322">
   <si>
     <t>Gene</t>
   </si>
@@ -963,21 +963,12 @@
     <t>Some prognostic effects in colon cancer and gastric cancer.  Activation may mediate resistance to EGFR TKIs, PI3K inhibitors, and AKT inhibitors. Activation may predict sensitivity to inhibitors of WNT signaling</t>
   </si>
   <si>
-    <t>in moalmanac</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
-    <t>Insufficient evidence for actionability</t>
-  </si>
-  <si>
     <t>CDK2 inhibitor</t>
   </si>
   <si>
-    <t>Molecular Oncology Almanac is not currently cataloging diagnostic assertions</t>
-  </si>
-  <si>
     <t>Partial keep</t>
   </si>
   <si>
@@ -990,9 +981,6 @@
     <t>Kept resistance assertion</t>
   </si>
   <si>
-    <t>Have a separate prognostic assertion</t>
-  </si>
-  <si>
     <t>Kept the prognostic assertion</t>
   </si>
   <si>
@@ -1005,9 +993,6 @@
     <t>Have separate assertions for AURKA inhibition</t>
   </si>
   <si>
-    <t>Molecular Oncology Almanac is not currently cataloging this type of assertion</t>
-  </si>
-  <si>
     <t>IDH inhibitors</t>
   </si>
   <si>
@@ -1018,6 +1003,24 @@
   </si>
   <si>
     <t>prognosis_n</t>
+  </si>
+  <si>
+    <t>included_in_lift_to_moalmanac</t>
+  </si>
+  <si>
+    <t>Unable to find supporting citation</t>
+  </si>
+  <si>
+    <t>Diagnostic assertions not cataloged by MOAlmanac</t>
+  </si>
+  <si>
+    <t>Assertion type not catalogued by MOAlmanac</t>
+  </si>
+  <si>
+    <t>incidental germline event</t>
+  </si>
+  <si>
+    <t>Diagnostic assertions not cataloged by MOAlmanac. Have a separate prognostic assertion</t>
   </si>
 </sst>
 </file>
@@ -1661,9 +1664,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1677,7 +1680,7 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1691,22 +1694,22 @@
         <v>221</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -1832,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -1933,7 +1936,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1976,7 +1979,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -1996,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -2079,7 +2082,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2099,7 +2102,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -2139,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.2">
@@ -2182,7 +2185,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2202,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2216,16 +2219,16 @@
         <v>19</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>51</v>
       </c>
@@ -2239,8 +2242,11 @@
       <c r="E27" s="1">
         <v>0</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>306</v>
+      <c r="F27" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -2280,7 +2286,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2300,7 +2306,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2320,7 +2326,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -2360,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2380,10 +2386,10 @@
         <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>63</v>
       </c>
@@ -2398,7 +2404,10 @@
         <v>0</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>306</v>
+        <v>319</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.2">
@@ -2438,10 +2447,10 @@
         <v>1</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="J37" s="1">
         <v>1</v>
@@ -2464,7 +2473,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -2484,10 +2493,10 @@
         <v>1</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="J39" s="1">
         <v>14</v>
@@ -2533,7 +2542,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2553,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -2613,7 +2622,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -2653,16 +2662,16 @@
         <v>1</v>
       </c>
       <c r="F47" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>310</v>
-      </c>
       <c r="I47" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>87</v>
       </c>
@@ -2676,11 +2685,14 @@
       <c r="E48" s="1">
         <v>0</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="F48" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>88</v>
       </c>
@@ -2694,11 +2706,14 @@
       <c r="E49" s="1">
         <v>0</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="F49" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>89</v>
       </c>
@@ -2712,11 +2727,14 @@
       <c r="E50" s="1">
         <v>0</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="F50" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>90</v>
       </c>
@@ -2730,11 +2748,14 @@
       <c r="E51" s="1">
         <v>0</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="F51" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="170" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>91</v>
       </c>
@@ -2748,11 +2769,11 @@
       <c r="E52" s="1">
         <v>0</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>306</v>
+      <c r="F52" s="5" t="s">
+        <v>319</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -2772,10 +2793,10 @@
         <v>1</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="J53" s="1">
         <v>2</v>
@@ -2901,7 +2922,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2921,7 +2942,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2941,7 +2962,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2961,7 +2982,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -2975,7 +2996,7 @@
         <v>7</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -2998,7 +3019,7 @@
         <v>7</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E64" s="1">
         <v>1</v>
@@ -3027,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3047,7 +3068,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -3087,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -3173,10 +3194,10 @@
         <v>0</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3194,7 +3215,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3214,7 +3235,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
@@ -3254,7 +3275,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3272,7 +3293,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -3315,7 +3336,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
@@ -3353,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
@@ -3429,7 +3450,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
@@ -3467,7 +3488,7 @@
         <v>0</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3487,7 +3508,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3505,7 +3526,7 @@
         <v>0</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3523,7 +3544,7 @@
         <v>0</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3543,7 +3564,7 @@
         <v>0</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3563,10 +3584,10 @@
         <v>0</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>168</v>
       </c>
@@ -3583,7 +3604,10 @@
         <v>0</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>306</v>
+        <v>319</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -3703,7 +3727,7 @@
         <v>0</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3723,7 +3747,7 @@
         <v>0</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="45" x14ac:dyDescent="0.2">
@@ -3783,7 +3807,7 @@
         <v>0</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -3803,10 +3827,10 @@
         <v>1</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="J104" s="1">
         <v>1</v>
@@ -3885,7 +3909,7 @@
         <v>0</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3903,7 +3927,7 @@
         <v>0</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="85" x14ac:dyDescent="0.2">
@@ -3923,10 +3947,10 @@
         <v>0</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="111" spans="1:10" ht="45" x14ac:dyDescent="0.2">
@@ -3946,7 +3970,7 @@
         <v>0</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="112" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3966,7 +3990,7 @@
         <v>0</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -3986,7 +4010,7 @@
         <v>0</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="114" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -4006,7 +4030,7 @@
         <v>0</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -4024,7 +4048,7 @@
         <v>0</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
@@ -4064,10 +4088,13 @@
         <v>281</v>
       </c>
       <c r="E117" s="1">
-        <v>0</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>304</v>
+        <v>1</v>
+      </c>
+      <c r="I117" s="1">
+        <v>5</v>
+      </c>
+      <c r="J117" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
@@ -4110,7 +4137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>214</v>
       </c>
@@ -4125,10 +4152,13 @@
         <v>0</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>319</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>215</v>
       </c>
@@ -4143,7 +4173,10 @@
         <v>0</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>316</v>
+        <v>319</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="122" spans="1:10" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -4163,11 +4196,11 @@
         <v>0</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D122">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D122">
     <sortCondition ref="A2:A122"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>